<commit_message>
feat: improve lat lng function
</commit_message>
<xml_diff>
--- a/Data/clean_data_sp_w_revenue_w_potential_w_latlng.xlsx
+++ b/Data/clean_data_sp_w_revenue_w_potential_w_latlng.xlsx
@@ -2018,10 +2018,10 @@
         </is>
       </c>
       <c r="AJ13" t="n">
-        <v>-23.911773</v>
+        <v>-23.581535</v>
       </c>
       <c r="AK13" t="n">
-        <v>-46.709817</v>
+        <v>-46.638664</v>
       </c>
     </row>
     <row r="14">
@@ -4358,10 +4358,10 @@
         </is>
       </c>
       <c r="AJ33" t="n">
-        <v>-23.569176</v>
+        <v>-23.574167</v>
       </c>
       <c r="AK33" t="n">
-        <v>-46.715102</v>
+        <v>-46.723611</v>
       </c>
     </row>
     <row r="34">
@@ -5294,10 +5294,10 @@
         </is>
       </c>
       <c r="AJ41" t="n">
-        <v>-23.53791</v>
+        <v>-23.548721</v>
       </c>
       <c r="AK41" t="n">
-        <v>-46.628445</v>
+        <v>-46.612418</v>
       </c>
     </row>
     <row r="42">
@@ -5528,10 +5528,10 @@
         </is>
       </c>
       <c r="AJ43" t="n">
-        <v>-22.994606</v>
+        <v>-23.586337</v>
       </c>
       <c r="AK43" t="n">
-        <v>-47.50946</v>
+        <v>-46.44503</v>
       </c>
     </row>
     <row r="44">
@@ -6230,10 +6230,10 @@
         </is>
       </c>
       <c r="AJ49" t="n">
-        <v>-23.674251</v>
+        <v>-23.537394</v>
       </c>
       <c r="AK49" t="n">
-        <v>-46.48769</v>
+        <v>-46.742615</v>
       </c>
     </row>
     <row r="50">
@@ -7517,10 +7517,10 @@
         </is>
       </c>
       <c r="AJ60" t="n">
-        <v>-23.121368</v>
+        <v>-23.610339</v>
       </c>
       <c r="AK60" t="n">
-        <v>-46.546356</v>
+        <v>-46.464257</v>
       </c>
     </row>
     <row r="61">
@@ -7985,10 +7985,10 @@
         </is>
       </c>
       <c r="AJ64" t="n">
-        <v>-23.555771</v>
+        <v>-23.554291</v>
       </c>
       <c r="AK64" t="n">
-        <v>-46.639557</v>
+        <v>-46.670987</v>
       </c>
     </row>
     <row r="65">
@@ -8804,10 +8804,10 @@
         </is>
       </c>
       <c r="AJ71" t="n">
-        <v>-23.462322</v>
+        <v>-23.874332</v>
       </c>
       <c r="AK71" t="n">
-        <v>-46.704409</v>
+        <v>-46.648936</v>
       </c>
     </row>
     <row r="72">
@@ -8921,10 +8921,10 @@
         </is>
       </c>
       <c r="AJ72" t="n">
-        <v>-23.469705</v>
+        <v>-23.489079</v>
       </c>
       <c r="AK72" t="n">
-        <v>-46.472079</v>
+        <v>-46.475063</v>
       </c>
     </row>
     <row r="73">
@@ -9155,10 +9155,10 @@
         </is>
       </c>
       <c r="AJ74" t="n">
-        <v>-23.555771</v>
+        <v>-23.528152</v>
       </c>
       <c r="AK74" t="n">
-        <v>-46.639557</v>
+        <v>-46.63366</v>
       </c>
     </row>
     <row r="75">
@@ -9389,10 +9389,10 @@
         </is>
       </c>
       <c r="AJ76" t="n">
-        <v>-23.619621</v>
+        <v>-23.619139</v>
       </c>
       <c r="AK76" t="n">
-        <v>-46.490532</v>
+        <v>-46.498064</v>
       </c>
     </row>
     <row r="77">
@@ -9857,10 +9857,10 @@
         </is>
       </c>
       <c r="AJ80" t="n">
-        <v>-23.543931</v>
+        <v>-23.543666</v>
       </c>
       <c r="AK80" t="n">
-        <v>-46.621694</v>
+        <v>-46.619619</v>
       </c>
     </row>
     <row r="81">
@@ -11027,10 +11027,10 @@
         </is>
       </c>
       <c r="AJ90" t="n">
-        <v>-23.618101</v>
+        <v>-22.420059</v>
       </c>
       <c r="AK90" t="n">
-        <v>-46.41713</v>
+        <v>-48.623028</v>
       </c>
     </row>
     <row r="91">
@@ -11144,10 +11144,10 @@
         </is>
       </c>
       <c r="AJ91" t="n">
-        <v>-21.154149</v>
+        <v>-23.498476</v>
       </c>
       <c r="AK91" t="n">
-        <v>-47.787355</v>
+        <v>-46.463266</v>
       </c>
     </row>
     <row r="92">
@@ -11612,10 +11612,10 @@
         </is>
       </c>
       <c r="AJ95" t="n">
-        <v>-23.469045</v>
+        <v>-23.500719</v>
       </c>
       <c r="AK95" t="n">
-        <v>-46.403396</v>
+        <v>-46.395185</v>
       </c>
     </row>
     <row r="96">
@@ -12080,10 +12080,10 @@
         </is>
       </c>
       <c r="AJ99" t="n">
-        <v>-23.755327</v>
+        <v>-23.779204</v>
       </c>
       <c r="AK99" t="n">
-        <v>-46.784744</v>
+        <v>-46.746414</v>
       </c>
     </row>
     <row r="100">
@@ -12314,10 +12314,10 @@
         </is>
       </c>
       <c r="AJ101" t="n">
-        <v>-21.755827</v>
+        <v>-23.573414</v>
       </c>
       <c r="AK101" t="n">
-        <v>-48.163521</v>
+        <v>-46.672948</v>
       </c>
     </row>
     <row r="102">
@@ -14303,10 +14303,10 @@
         </is>
       </c>
       <c r="AJ118" t="n">
-        <v>-23.555771</v>
+        <v>-23.573414</v>
       </c>
       <c r="AK118" t="n">
-        <v>-46.639557</v>
+        <v>-46.672948</v>
       </c>
     </row>
     <row r="119">
@@ -15122,10 +15122,10 @@
         </is>
       </c>
       <c r="AJ125" t="n">
-        <v>-23.473794</v>
+        <v>-23.464462</v>
       </c>
       <c r="AK125" t="n">
-        <v>-47.445363</v>
+        <v>-46.405074</v>
       </c>
     </row>
     <row r="126">
@@ -15941,10 +15941,10 @@
         </is>
       </c>
       <c r="AJ132" t="n">
-        <v>-23.555771</v>
+        <v>-23.620853</v>
       </c>
       <c r="AK132" t="n">
-        <v>-46.639557</v>
+        <v>-46.613832</v>
       </c>
     </row>
     <row r="133">
@@ -16994,10 +16994,10 @@
         </is>
       </c>
       <c r="AJ141" t="n">
-        <v>-23.940272</v>
+        <v>-23.584632</v>
       </c>
       <c r="AK141" t="n">
-        <v>-46.394549</v>
+        <v>-46.695629</v>
       </c>
     </row>
     <row r="142">
@@ -18515,10 +18515,10 @@
         </is>
       </c>
       <c r="AJ154" t="n">
-        <v>-23.906403</v>
+        <v>-23.907276</v>
       </c>
       <c r="AK154" t="n">
-        <v>-46.707666</v>
+        <v>-46.706429</v>
       </c>
     </row>
     <row r="155">
@@ -18983,10 +18983,10 @@
         </is>
       </c>
       <c r="AJ158" t="n">
-        <v>-21.131898</v>
+        <v>-23.607064</v>
       </c>
       <c r="AK158" t="n">
-        <v>-51.10187</v>
+        <v>-46.642778</v>
       </c>
     </row>
     <row r="159">
@@ -19802,10 +19802,10 @@
         </is>
       </c>
       <c r="AJ165" t="n">
-        <v>-23.566413</v>
+        <v>-23.58208</v>
       </c>
       <c r="AK165" t="n">
-        <v>-46.588119</v>
+        <v>-46.561689</v>
       </c>
     </row>
     <row r="166">
@@ -20153,10 +20153,10 @@
         </is>
       </c>
       <c r="AJ168" t="n">
-        <v>-23.462352</v>
+        <v>-23.4697</v>
       </c>
       <c r="AK168" t="n">
-        <v>-46.608406</v>
+        <v>-46.614811</v>
       </c>
     </row>
     <row r="169">
@@ -20270,10 +20270,10 @@
         </is>
       </c>
       <c r="AJ169" t="n">
-        <v>-23.568528</v>
+        <v>-23.530429</v>
       </c>
       <c r="AK169" t="n">
-        <v>-46.658143</v>
+        <v>-46.421988</v>
       </c>
     </row>
     <row r="170">
@@ -22727,10 +22727,10 @@
         </is>
       </c>
       <c r="AJ190" t="n">
-        <v>-23.276274</v>
+        <v>-23.701697</v>
       </c>
       <c r="AK190" t="n">
-        <v>-45.842213</v>
+        <v>-46.705899</v>
       </c>
     </row>
     <row r="191">
@@ -25652,10 +25652,10 @@
         </is>
       </c>
       <c r="AJ215" t="n">
-        <v>-22.25</v>
+        <v>-23.545108</v>
       </c>
       <c r="AK215" t="n">
-        <v>-47.483333</v>
+        <v>-46.642778</v>
       </c>
     </row>
     <row r="216">
@@ -26003,10 +26003,10 @@
         </is>
       </c>
       <c r="AJ218" t="n">
-        <v>-23.555771</v>
+        <v>-23.724654</v>
       </c>
       <c r="AK218" t="n">
-        <v>-46.639557</v>
+        <v>-49.425075</v>
       </c>
     </row>
     <row r="219">
@@ -26120,10 +26120,10 @@
         </is>
       </c>
       <c r="AJ219" t="n">
-        <v>-23.803515</v>
+        <v>-23.690936</v>
       </c>
       <c r="AK219" t="n">
-        <v>-46.021825</v>
+        <v>-46.751724</v>
       </c>
     </row>
     <row r="220">
@@ -26588,10 +26588,10 @@
         </is>
       </c>
       <c r="AJ223" t="n">
-        <v>-23.243081</v>
+        <v>-23.867908</v>
       </c>
       <c r="AK223" t="n">
-        <v>-46.889499</v>
+        <v>-46.736352</v>
       </c>
     </row>
     <row r="224">
@@ -27173,10 +27173,10 @@
         </is>
       </c>
       <c r="AJ228" t="n">
-        <v>-23.498996</v>
+        <v>-23.493039</v>
       </c>
       <c r="AK228" t="n">
-        <v>-46.625592</v>
+        <v>-46.626368</v>
       </c>
     </row>
     <row r="229">
@@ -28694,10 +28694,10 @@
         </is>
       </c>
       <c r="AJ241" t="n">
-        <v>-22.961588</v>
+        <v>-23.459863</v>
       </c>
       <c r="AK241" t="n">
-        <v>-45.545345</v>
+        <v>-46.625474</v>
       </c>
     </row>
     <row r="242">
@@ -30215,10 +30215,10 @@
         </is>
       </c>
       <c r="AJ254" t="n">
-        <v>-23.55063</v>
+        <v>-23.551636</v>
       </c>
       <c r="AK254" t="n">
-        <v>-46.538291</v>
+        <v>-46.536032</v>
       </c>
     </row>
     <row r="255">
@@ -33842,10 +33842,10 @@
         </is>
       </c>
       <c r="AJ285" t="n">
-        <v>-21.274345</v>
+        <v>-23.470526</v>
       </c>
       <c r="AK285" t="n">
-        <v>-47.304775</v>
+        <v>-46.673552</v>
       </c>
     </row>
     <row r="286">
@@ -34661,10 +34661,10 @@
         </is>
       </c>
       <c r="AJ292" t="n">
-        <v>-23.173531</v>
+        <v>-23.45697</v>
       </c>
       <c r="AK292" t="n">
-        <v>-45.879069</v>
+        <v>-46.696494</v>
       </c>
     </row>
     <row r="293">
@@ -34895,10 +34895,10 @@
         </is>
       </c>
       <c r="AJ294" t="n">
-        <v>-23.443682</v>
+        <v>-23.543197</v>
       </c>
       <c r="AK294" t="n">
-        <v>-46.694681</v>
+        <v>-46.577774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>